<commit_message>
adding anomaly regression code
</commit_message>
<xml_diff>
--- a/IdealDataSetOutline.xlsx
+++ b/IdealDataSetOutline.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenahorton/Documents/HBS/ESE 168/ESE168_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D9994F8-E86C-F643-AF3E-0A5501A41E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA22CF1-06B4-4F45-8F95-CD281B1ED9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="2360" windowWidth="24840" windowHeight="13440" xr2:uid="{ABCADE8A-B2D9-CE40-83D6-7A5D26B529E4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{ABCADE8A-B2D9-CE40-83D6-7A5D26B529E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Year</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>&lt;&lt;--- and include time shifted variables of each of these</t>
+  </si>
+  <si>
+    <t>% Change in Major Exporter's Production</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D144BD1-2D37-8D45-AE74-E930DCC66C93}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,10 +436,11 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,9 +460,12 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>